<commit_message>
migracion datos jetperu 01
</commit_message>
<xml_diff>
--- a/uploads/Reporte JET PERU.xlsx
+++ b/uploads/Reporte JET PERU.xlsx
@@ -144,10 +144,10 @@
     <t>Tipo Transferencia</t>
   </si>
   <si>
-    <t>.15.12.2022</t>
-  </si>
-  <si>
-    <t>.16.12.2022</t>
+    <t>.12.15.2022</t>
+  </si>
+  <si>
+    <t>.13.12.2022</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
     <col min="6" max="6" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="3" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -658,7 +658,7 @@
         <v>1243333333</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
+        <v>500.5</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>22</v>
@@ -717,7 +717,7 @@
         <v>9876543</v>
       </c>
       <c r="I3" s="4">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>28</v>
@@ -776,7 +776,7 @@
         <v>9876543</v>
       </c>
       <c r="I4" s="4">
-        <v>0</v>
+        <v>1500.9</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
migracion datos jetperu y tpp OK
</commit_message>
<xml_diff>
--- a/uploads/Reporte JET PERU.xlsx
+++ b/uploads/Reporte JET PERU.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>Fecha</t>
   </si>
@@ -144,17 +144,29 @@
     <t>Tipo Transferencia</t>
   </si>
   <si>
-    <t>.12.15.2022</t>
-  </si>
-  <si>
     <t>.13.12.2022</t>
+  </si>
+  <si>
+    <t>.15.12.2022</t>
+  </si>
+  <si>
+    <t>.06.02.2021</t>
+  </si>
+  <si>
+    <t>.13.07.2021</t>
+  </si>
+  <si>
+    <t>.11.02.2021</t>
+  </si>
+  <si>
+    <t>.15.07.2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,14 +183,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -206,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -224,9 +228,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -543,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -752,7 +753,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -785,7 +786,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>30</v>
@@ -810,7 +811,181 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5409</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1243333333</v>
+      </c>
+      <c r="I5" s="4">
+        <v>500.5</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.50050925925925926</v>
+      </c>
+      <c r="N5" s="3">
+        <v>99999999</v>
+      </c>
+      <c r="O5" s="3">
+        <v>797453</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5410</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9876543</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="3">
+        <v>918881831</v>
+      </c>
+      <c r="O6" s="3">
+        <v>797453</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5410</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3">
+        <v>9876543</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1500.9</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="3">
+        <v>918881831</v>
+      </c>
+      <c r="O7" s="3">
+        <v>797453</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>